<commit_message>
After excel for both
</commit_message>
<xml_diff>
--- a/excelfortest.xlsx
+++ b/excelfortest.xlsx
@@ -4,35 +4,54 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Output" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Praveen</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>gi</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>support@z4.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>pageName</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,13 +59,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -58,13 +105,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,31 +424,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"Chrome, internet, Firefox"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"working, prod"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>